<commit_message>
changed emilys sheet to show what to do
</commit_message>
<xml_diff>
--- a/data/emily_harders/Experiment3_corttimecourse_datasheet_1Feb22 - Sheet9.xlsx
+++ b/data/emily_harders/Experiment3_corttimecourse_datasheet_1Feb22 - Sheet9.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wlperry/Documents/R Projects/R_fun_time/data/emily_harders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{565DFCDA-ED41-FA4D-A0D6-BABFE7844711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83ADE80F-DDF6-C143-B6F2-A79218E165A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment3_corttimecourse_data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="11">
   <si>
     <t>EggID</t>
   </si>
@@ -51,11 +51,14 @@
   <si>
     <t>oil</t>
   </si>
+  <si>
+    <t>expression over time</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -889,11 +892,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -906,9 +909,10 @@
     <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -934,7 +938,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3</v>
       </c>
@@ -959,8 +963,11 @@
       <c r="H2">
         <v>0.70699182000000005</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>4</v>
       </c>
@@ -986,7 +993,7 @@
         <v>0.69983580599999995</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>6</v>
       </c>
@@ -1012,7 +1019,7 @@
         <v>0.70664719200000004</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>8</v>
       </c>
@@ -1038,7 +1045,7 @@
         <v>0.70664719200000004</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>11</v>
       </c>
@@ -1064,7 +1071,7 @@
         <v>0.70527252399999996</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>12</v>
       </c>
@@ -1090,7 +1097,7 @@
         <v>0.70664719200000004</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>15</v>
       </c>
@@ -1116,7 +1123,7 @@
         <v>0.70699182000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>16</v>
       </c>
@@ -1142,7 +1149,7 @@
         <v>0.70664719200000004</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>19</v>
       </c>
@@ -1168,7 +1175,7 @@
         <v>0.70664719200000004</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>21</v>
       </c>
@@ -1194,7 +1201,7 @@
         <v>0.70527252399999996</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>22</v>
       </c>
@@ -1220,7 +1227,7 @@
         <v>0.70527252399999996</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>23</v>
       </c>
@@ -1246,7 +1253,7 @@
         <v>0.69983580599999995</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>25</v>
       </c>
@@ -1272,7 +1279,7 @@
         <v>0.70527252399999996</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>27</v>
       </c>
@@ -1298,7 +1305,7 @@
         <v>0.70699182000000005</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>28</v>
       </c>

</xml_diff>